<commit_message>
Mise à jour de la DocTechique, ajout d'un fichier excel pour les Test
</commit_message>
<xml_diff>
--- a/Documentation/PlanifDetail.xlsx
+++ b/Documentation/PlanifDetail.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\TPI\CloneRepo\sadekTPI\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initial" sheetId="1" r:id="rId1"/>
     <sheet name="Réel" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +108,13 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
@@ -396,6 +398,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +707,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -710,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:CE22"/>
+  <dimension ref="B2:CE20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AO24" sqref="AO24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,16 +1872,16 @@
       <c r="CD15" s="12"/>
       <c r="CE15" s="14"/>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C17" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="X22" s="2"/>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1886,10 +1891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:CE22"/>
+  <dimension ref="B2:CE20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="BK23" sqref="BK23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2273,7 @@
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="27"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -2674,30 +2679,30 @@
       <c r="BE11" s="12"/>
       <c r="BF11" s="12"/>
       <c r="BG11" s="12"/>
-      <c r="BH11" s="9"/>
-      <c r="BI11" s="9"/>
-      <c r="BJ11" s="9"/>
-      <c r="BK11" s="9"/>
-      <c r="BL11" s="9"/>
-      <c r="BM11" s="9"/>
-      <c r="BN11" s="9"/>
-      <c r="BO11" s="9"/>
-      <c r="BP11" s="9"/>
-      <c r="BQ11" s="9"/>
-      <c r="BR11" s="9"/>
-      <c r="BS11" s="9"/>
-      <c r="BT11" s="9"/>
-      <c r="BU11" s="9"/>
-      <c r="BV11" s="9"/>
-      <c r="BW11" s="9"/>
-      <c r="BX11" s="9"/>
-      <c r="BY11" s="9"/>
-      <c r="BZ11" s="9"/>
-      <c r="CA11" s="9"/>
-      <c r="CB11" s="9"/>
-      <c r="CC11" s="9"/>
-      <c r="CD11" s="9"/>
-      <c r="CE11" s="10"/>
+      <c r="BH11" s="28"/>
+      <c r="BI11" s="28"/>
+      <c r="BJ11" s="28"/>
+      <c r="BK11" s="28"/>
+      <c r="BL11" s="28"/>
+      <c r="BM11" s="28"/>
+      <c r="BN11" s="28"/>
+      <c r="BO11" s="28"/>
+      <c r="BP11" s="28"/>
+      <c r="BQ11" s="28"/>
+      <c r="BR11" s="28"/>
+      <c r="BS11" s="28"/>
+      <c r="BT11" s="28"/>
+      <c r="BU11" s="28"/>
+      <c r="BV11" s="28"/>
+      <c r="BW11" s="28"/>
+      <c r="BX11" s="28"/>
+      <c r="BY11" s="28"/>
+      <c r="BZ11" s="28"/>
+      <c r="CA11" s="28"/>
+      <c r="CB11" s="28"/>
+      <c r="CC11" s="28"/>
+      <c r="CD11" s="28"/>
+      <c r="CE11" s="29"/>
     </row>
     <row r="12" spans="2:83" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
@@ -3043,16 +3048,16 @@
       <c r="CD15" s="12"/>
       <c r="CE15" s="14"/>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C17" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="X22" s="2"/>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="X20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>